<commit_message>
adding frame length to grid, correcting unit conversions for media
</commit_message>
<xml_diff>
--- a/frameList.xlsx
+++ b/frameList.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.56000000000000005</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>